<commit_message>
fix: bugs and timeout
</commit_message>
<xml_diff>
--- a/RemoverGrupo.xlsx
+++ b/RemoverGrupo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScopeAutomations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD11441-1095-4B6B-99C0-CFCCEFE31B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC5896C-B431-4B04-B0C6-AB498C898BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EF43BA7A-AC6D-4730-9109-E31FF2513008}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{EF43BA7A-AC6D-4730-9109-E31FF2513008}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,36 +36,309 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>8AP359ATNPU302967</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU302977</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU303700</t>
-  </si>
-  <si>
-    <t>93YRBB002RJ773959</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU300121</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU300319</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU300389</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU304822</t>
-  </si>
-  <si>
-    <t>8AP359ATNPU305523</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
   <si>
     <t>CHASSI</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774458</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774489</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774539</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774668</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774699</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774704</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ774766</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ794967</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ794998</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795035</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795097</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795133</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795245</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795293</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795326</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795388</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795438</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795455</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795584</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795603</t>
+  </si>
+  <si>
+    <t>93YRBB007RJ795679</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ772296</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ772430</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774453</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774503</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774520</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774727</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774789</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774792</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774887</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774890</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ774954</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ772338</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ773697</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774493</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774512</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774557</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774588</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774591</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774610</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774655</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ774686</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ795523</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774471</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774485</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774499</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774518</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774535</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774597</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774616</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774664</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774714</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774728</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774745</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774759</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774793</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774809</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774812</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774826</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774843</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774860</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774874</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774888</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774891</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774924</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774969</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ774972</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ795529</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ795630</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ795644</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ795725</t>
+  </si>
+  <si>
+    <t>93YRBB00XRJ795787</t>
+  </si>
+  <si>
+    <t>93YRBB004RJ588442</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ588260</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ588436</t>
+  </si>
+  <si>
+    <t>93YRBB00XPJ405512</t>
+  </si>
+  <si>
+    <t>93YRBB00XPJ405560</t>
+  </si>
+  <si>
+    <t>93YRBB003RJ591963</t>
+  </si>
+  <si>
+    <t>93YRBB004RJ588294</t>
+  </si>
+  <si>
+    <t>93YRBB004RJ588604</t>
+  </si>
+  <si>
+    <t>93YRBB007PJ302466</t>
+  </si>
+  <si>
+    <t>93YRBB008RJ587861</t>
+  </si>
+  <si>
+    <t>93YRBB009RJ588226</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ772275</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ772308</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ774429</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ774477</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ774513</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ774530</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ774723</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ794891</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ795037</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ795085</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ795328</t>
+  </si>
+  <si>
+    <t>93YRBB000RJ795782</t>
+  </si>
+  <si>
+    <t>93YRBB001RJ733811</t>
+  </si>
+  <si>
+    <t>93YRBB001RJ772107</t>
+  </si>
+  <si>
+    <t>93YRBB001RJ772124</t>
+  </si>
+  <si>
+    <t>93YRBB001RJ772155</t>
+  </si>
+  <si>
+    <t>93YRBB001RJ772219</t>
   </si>
 </sst>
 </file>
@@ -124,7 +397,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -440,65 +713,520 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E1FC7A-A22E-497B-9938-4D43E8448528}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>